<commit_message>
feat: add aging proccess
</commit_message>
<xml_diff>
--- a/projection/csv/bazneshaste_bimepardaz_just_all.xlsx
+++ b/projection/csv/bazneshaste_bimepardaz_just_all.xlsx
@@ -22,7 +22,7 @@
     <t>average_salary</t>
   </si>
   <si>
-    <t>average_insurance_record</t>
+    <t>insurance_record</t>
   </si>
   <si>
     <t>number</t>
@@ -43,7 +43,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -424,7 +424,7 @@
     <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>